<commit_message>
last commit before manual review with sjshaw
</commit_message>
<xml_diff>
--- a/docs/new_schema_error_reports.xlsx
+++ b/docs/new_schema_error_reports.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="old_data_vs_new_schema" sheetId="3" r:id="rId1"/>
@@ -2440,8 +2440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3442,8 +3442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>